<commit_message>
new commit 21/3 1
</commit_message>
<xml_diff>
--- a/Stargems/Data/Data.xlsx
+++ b/Stargems/Data/Data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/eclipse-workspace/Stargems/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/git/StargemsWEB/Stargems/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37398B8B-99A8-9A47-9C4B-344B775184FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C472CF0-B864-014D-97F2-21B55A26E68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22320" windowHeight="15800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22320" windowHeight="15740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>amagsh@1232</t>
   </si>
@@ -147,6 +148,18 @@
   </si>
   <si>
     <t>1232654500</t>
+  </si>
+  <si>
+    <t>Amar</t>
+  </si>
+  <si>
+    <t>Kadam</t>
+  </si>
+  <si>
+    <t>amar.kadam@openxcell.com</t>
+  </si>
+  <si>
+    <t>Amar@1234</t>
   </si>
 </sst>
 </file>
@@ -559,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCC6F12-DAF9-B840-8EBF-A49D6D0C015E}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -621,4 +634,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7907A463-E236-7E4E-A428-0C2412336C57}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{5F016C19-6DB9-E948-B6CF-0748919ACABF}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{08B72E2D-49A6-6645-B418-160FB97EBC40}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{3C5E3D19-9588-E143-8C60-31C7A0CB2183}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>